<commit_message>
update pelengkapan fitur fac
</commit_message>
<xml_diff>
--- a/excel/riwayat_donasi_4_2023-06-12.xlsx
+++ b/excel/riwayat_donasi_4_2023-06-12.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>Riwayat ID</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>kartu_kredit</t>
+  </si>
+  <si>
+    <t>denny ariyana</t>
   </si>
 </sst>
 </file>
@@ -393,7 +396,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -732,6 +735,52 @@
         <v>9</v>
       </c>
     </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>72</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>300000</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <v>73</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>1500000</v>
+      </c>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>